<commit_message>
Diane's correction prior to discussion
</commit_message>
<xml_diff>
--- a/resources/acronyms.xlsx
+++ b/resources/acronyms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27004"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreas/projects/g2sq/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{41695949-252A-554F-B078-FF69E322F75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32102139-5CDA-4CDC-8C79-6DCA5B37DA1A}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{41695949-252A-554F-B078-FF69E322F75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECD2A4BF-D4C5-4583-A9B8-9AAE05798ADD}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="23260" windowHeight="12580" xr2:uid="{5F610E7D-516F-4D0E-9C99-25E102E12365}"/>
   </bookViews>
@@ -47,13 +47,13 @@
     <t>LSMS</t>
   </si>
   <si>
-    <t>Living Standard Measurement Survey</t>
+    <t>Living Standards Measurement Survey</t>
   </si>
   <si>
     <t>CAPI</t>
   </si>
   <si>
-    <t>Computer Assissted Personal Interviewing</t>
+    <t>Computer Assisted Personal Interviewing</t>
   </si>
   <si>
     <t>NSO</t>
@@ -77,7 +77,7 @@
     <t>CATI</t>
   </si>
   <si>
-    <t>Computer Assissted Telephone Interviewing</t>
+    <t>Computer Assisted Telephone Interviewing</t>
   </si>
   <si>
     <t>PAPI</t>
@@ -113,7 +113,7 @@
     <t>ToC</t>
   </si>
   <si>
-    <t>Table of Content</t>
+    <t>Table of Contents</t>
   </si>
   <si>
     <t>HIES</t>
@@ -125,7 +125,7 @@
     <t>CAWI</t>
   </si>
   <si>
-    <t>Computer Assissted Web Interviewing</t>
+    <t>Computer Assisted Web Interviewing</t>
   </si>
   <si>
     <t>EA</t>
@@ -504,7 +504,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>